<commit_message>
Added 0.1 Threshold into Classification Report
</commit_message>
<xml_diff>
--- a/Datasets/Calculation Result/Classification Report/Classification Report TB - Stanford comparison.xlsx
+++ b/Datasets/Calculation Result/Classification Report/Classification Report TB - Stanford comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Calculation Result\Classification Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E33ED3-3BDC-49B8-B8AD-EECC19B66E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A50CA94-BD2A-415B-89DE-0701580C08F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{356F8004-839F-4170-968A-E905A86D7A5F}"/>
+    <workbookView xWindow="15600" yWindow="3435" windowWidth="20910" windowHeight="11835" xr2:uid="{356F8004-839F-4170-968A-E905A86D7A5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="91">
   <si>
     <t>Stanford</t>
   </si>
@@ -86,9 +86,6 @@
     <t>0.04</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
     <t>Neutral Class has no true samples hence N/A. Scikit learn solves it with output = 0.00</t>
   </si>
   <si>
@@ -116,24 +113,9 @@
     <t>0.07</t>
   </si>
   <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>0.61</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
     <t>0.91</t>
   </si>
   <si>
-    <t>0.94</t>
-  </si>
-  <si>
-    <t>0.10</t>
-  </si>
-  <si>
     <t>0.18</t>
   </si>
   <si>
@@ -146,21 +128,12 @@
     <t>0.65</t>
   </si>
   <si>
-    <t>0.97</t>
-  </si>
-  <si>
     <t>0.19</t>
   </si>
   <si>
     <t>0.96</t>
   </si>
   <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.56</t>
-  </si>
-  <si>
     <t>0.92</t>
   </si>
   <si>
@@ -182,21 +155,12 @@
     <t>0.43</t>
   </si>
   <si>
-    <t>0.17</t>
-  </si>
-  <si>
-    <t>0.28</t>
-  </si>
-  <si>
     <t>0.88</t>
   </si>
   <si>
     <t>0.58</t>
   </si>
   <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>0.64</t>
   </si>
   <si>
@@ -299,7 +263,49 @@
     <t>0.55</t>
   </si>
   <si>
-    <t>Textblob .5 Threshold</t>
+    <t>Textblob .3 Threshold</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.27</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.32</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -359,6 +365,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,7 +380,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,70 +699,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7679C0-E6FB-4780-AA1A-EA6D9AA2FADC}">
   <dimension ref="A1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="2"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
       <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="2"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
+      <c r="F3" s="15"/>
+      <c r="G3" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -761,108 +776,108 @@
       <c r="L3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="10"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="3">
+      <c r="D4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="10">
         <v>504</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="13"/>
       <c r="O4" s="3">
         <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="3">
+      <c r="C5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="10">
         <v>496</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="N5" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="13"/>
       <c r="O5" s="3">
         <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="3">
+      <c r="C6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="10">
         <v>504</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
@@ -872,24 +887,24 @@
       <c r="L6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="10"/>
+      <c r="M6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="13"/>
       <c r="O6" s="3">
         <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -898,116 +913,116 @@
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="10">
         <v>1000</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="N8" s="10"/>
+      <c r="M8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8" s="13"/>
       <c r="O8" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="10">
         <v>1000</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="N9" s="10"/>
+        <v>48</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="13"/>
       <c r="O9" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="3">
+      <c r="E10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="10">
         <v>1000</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="9"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="N10" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="13"/>
       <c r="O10" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1018,27 +1033,27 @@
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="3" t="s">
-        <v>19</v>
+      <c r="F12" s="15"/>
+      <c r="G12" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -1050,108 +1065,108 @@
       <c r="L12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N12" s="10"/>
+      <c r="N12" s="13"/>
       <c r="O12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="3">
+      <c r="C13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="10">
         <v>498</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="12"/>
       <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M13" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N13" s="10"/>
+        <v>52</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="13"/>
       <c r="O13" s="3">
         <v>498</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="3">
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="10">
         <v>498</v>
       </c>
       <c r="H14" s="2"/>
-      <c r="I14" s="9"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" s="10"/>
+        <v>55</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" s="13"/>
       <c r="O14" s="3">
         <v>498</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3">
+      <c r="C15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="10">
         <v>0</v>
       </c>
       <c r="H15" s="2"/>
-      <c r="I15" s="9"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1161,24 +1176,24 @@
       <c r="L15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="10"/>
+      <c r="M15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="13"/>
       <c r="O15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1187,116 +1202,116 @@
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="10">
         <v>996</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="9"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="N17" s="10"/>
+      <c r="M17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="13"/>
       <c r="O17" s="3">
         <v>996</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="10">
+        <v>996</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M18" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="3">
-        <v>996</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="N18" s="10"/>
+      <c r="N18" s="13"/>
       <c r="O18" s="3">
         <v>996</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="15"/>
+      <c r="G19" s="10">
         <v>996</v>
       </c>
       <c r="H19" s="2"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="N19" s="10"/>
+        <v>56</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" s="13"/>
       <c r="O19" s="3">
         <v>996</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1307,27 +1322,27 @@
       <c r="O20" s="2"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="3" t="s">
-        <v>19</v>
+      <c r="F21" s="15"/>
+      <c r="G21" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="12" t="s">
         <v>11</v>
       </c>
       <c r="J21" s="2" t="s">
@@ -1339,106 +1354,106 @@
       <c r="L21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="M21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N21" s="10"/>
+      <c r="N21" s="13"/>
       <c r="O21" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="3">
+      <c r="C22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="10">
         <v>500</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="9"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N22" s="10"/>
+        <v>61</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" s="13"/>
       <c r="O22" s="3">
         <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="2" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="3">
+      <c r="C23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="10">
         <v>500</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="9"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="M23" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N23" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="13"/>
       <c r="O23" s="3">
         <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="2" t="s">
+      <c r="A24" s="16"/>
+      <c r="B24" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="3"/>
+      <c r="C24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="9"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1448,22 +1463,22 @@
       <c r="L24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N24" s="10"/>
+      <c r="M24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="13"/>
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="9"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1472,116 +1487,116 @@
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="10">
         <v>1000</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="9"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="N26" s="10"/>
+      <c r="M26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="N26" s="13"/>
       <c r="O26" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="15"/>
+      <c r="G27" s="10">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="3">
-        <v>1000</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="L27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="N27" s="10"/>
+        <v>66</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="13"/>
       <c r="O27" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="3">
+      <c r="A28" s="16"/>
+      <c r="B28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="15"/>
+      <c r="G28" s="10">
         <v>1000</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="9"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="10"/>
+        <v>65</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N28" s="13"/>
       <c r="O28" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1592,27 +1607,27 @@
       <c r="O29" s="2"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="3" t="s">
-        <v>19</v>
+      <c r="F30" s="14"/>
+      <c r="G30" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="12" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="4" t="s">
@@ -1624,108 +1639,108 @@
       <c r="L30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="11" t="s">
+      <c r="M30" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="11"/>
+      <c r="N30" s="14"/>
       <c r="O30" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31">
+      <c r="C31" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="9">
         <v>167</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="9"/>
+      <c r="I31" s="12"/>
       <c r="J31" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="N31" s="12"/>
+        <v>20</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="N31" s="15"/>
       <c r="O31" s="4">
         <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F32" s="12"/>
-      <c r="G32">
+      <c r="C32" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="9">
         <v>769</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="9"/>
+      <c r="I32" s="12"/>
       <c r="J32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M32" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N32" s="12"/>
+        <v>43</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N32" s="15"/>
       <c r="O32" s="4">
         <v>769</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" t="s">
+      <c r="A33" s="16"/>
+      <c r="B33" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33">
+      <c r="C33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="15"/>
+      <c r="G33" s="9">
         <v>0</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="9"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="4" t="s">
         <v>8</v>
       </c>
@@ -1735,20 +1750,24 @@
       <c r="L33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="N33" s="12"/>
+      <c r="M33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="15"/>
       <c r="O33" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="9"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1757,114 +1776,116 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35">
+      <c r="A35" s="16"/>
+      <c r="B35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="15"/>
+      <c r="G35" s="9">
         <v>936</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="9"/>
+      <c r="I35" s="12"/>
       <c r="J35" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="N35" s="12"/>
+      <c r="M35" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N35" s="15"/>
       <c r="O35" s="4">
         <v>936</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36">
+      <c r="A36" s="16"/>
+      <c r="B36" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="15"/>
+      <c r="G36" s="9">
         <v>936</v>
       </c>
       <c r="H36" s="2"/>
-      <c r="I36" s="9"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="N36" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="N36" s="15"/>
       <c r="O36" s="4">
         <v>936</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37">
+      <c r="A37" s="16"/>
+      <c r="B37" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="9">
         <v>936</v>
       </c>
       <c r="H37" s="2"/>
-      <c r="I37" s="9"/>
+      <c r="I37" s="12"/>
       <c r="J37" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="M37" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="N37" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N37" s="15"/>
       <c r="O37" s="4">
         <v>936</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1875,27 +1896,27 @@
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="3" t="s">
-        <v>19</v>
+      <c r="F39" s="15"/>
+      <c r="G39" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="9" t="s">
+      <c r="I39" s="12" t="s">
         <v>13</v>
       </c>
       <c r="J39" s="2" t="s">
@@ -1907,108 +1928,108 @@
       <c r="L39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M39" s="10" t="s">
+      <c r="M39" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="N39" s="10"/>
+      <c r="N39" s="13"/>
       <c r="O39" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="2" t="s">
+      <c r="A40" s="16"/>
+      <c r="B40" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="3">
+      <c r="D40" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="10">
         <v>483</v>
       </c>
       <c r="H40" s="2"/>
-      <c r="I40" s="9"/>
+      <c r="I40" s="12"/>
       <c r="J40" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="M40" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="N40" s="10"/>
+      <c r="N40" s="13"/>
       <c r="O40" s="3">
         <v>483</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="2" t="s">
+      <c r="A41" s="16"/>
+      <c r="B41" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="3">
+      <c r="D41" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="15"/>
+      <c r="G41" s="10">
         <v>517</v>
       </c>
       <c r="H41" s="2"/>
-      <c r="I41" s="9"/>
+      <c r="I41" s="12"/>
       <c r="J41" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M41" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="N41" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="N41" s="13"/>
       <c r="O41" s="3">
         <v>517</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="16"/>
+      <c r="B42" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="3">
+      <c r="C42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="15"/>
+      <c r="G42" s="10">
         <v>0</v>
       </c>
       <c r="H42" s="2"/>
-      <c r="I42" s="9"/>
+      <c r="I42" s="12"/>
       <c r="J42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2018,24 +2039,24 @@
       <c r="L42" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M42" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="N42" s="10"/>
+      <c r="M42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N42" s="13"/>
       <c r="O42" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
       <c r="H43" s="2"/>
-      <c r="I43" s="9"/>
+      <c r="I43" s="12"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2044,120 +2065,120 @@
       <c r="O43" s="3"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="15"/>
+      <c r="G44" s="10">
         <v>1000</v>
       </c>
       <c r="H44" s="2"/>
-      <c r="I44" s="9"/>
+      <c r="I44" s="12"/>
       <c r="J44" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N44" s="10"/>
+      <c r="M44" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="N44" s="13"/>
       <c r="O44" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="3">
+      <c r="A45" s="16"/>
+      <c r="B45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="15"/>
+      <c r="G45" s="10">
         <v>1000</v>
       </c>
       <c r="H45" s="2"/>
-      <c r="I45" s="9"/>
+      <c r="I45" s="12"/>
       <c r="J45" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M45" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="N45" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N45" s="13"/>
       <c r="O45" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
-      <c r="B46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="3">
+      <c r="A46" s="16"/>
+      <c r="B46" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="10">
         <v>1000</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="I46" s="9"/>
+      <c r="I46" s="12"/>
       <c r="J46" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M46" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="N46" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="M46" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N46" s="13"/>
       <c r="O46" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
+      <c r="A49" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -2178,43 +2199,43 @@
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+      <c r="A55" s="11"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="11"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2223,30 +2244,30 @@
       <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
+      <c r="A58" s="11"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2259,43 +2280,43 @@
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2304,30 +2325,30 @@
       <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
       <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
-      <c r="E68" s="10"/>
-      <c r="F68" s="10"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
       <c r="G68" s="5"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
-      <c r="E69" s="10"/>
-      <c r="F69" s="10"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,8 +2365,8 @@
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -2353,8 +2374,8 @@
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -2362,8 +2383,8 @@
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
       <c r="G73" s="5"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2371,8 +2392,8 @@
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2389,8 +2410,8 @@
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2398,8 +2419,8 @@
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,8 +2428,8 @@
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -2425,8 +2446,8 @@
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2434,8 +2455,8 @@
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
       <c r="G81" s="7"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2443,8 +2464,8 @@
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
       <c r="G82" s="7"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2452,8 +2473,8 @@
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2470,8 +2491,8 @@
       <c r="B85" s="2"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2479,8 +2500,8 @@
       <c r="B86" s="2"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
       <c r="G86" s="7"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2488,8 +2509,8 @@
       <c r="B87" s="2"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
       <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2506,8 +2527,8 @@
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
       <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2515,8 +2536,8 @@
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2524,8 +2545,8 @@
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
-      <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,8 +2554,8 @@
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2551,8 +2572,8 @@
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="10"/>
-      <c r="F94" s="10"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
       <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2560,8 +2581,8 @@
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="10"/>
-      <c r="F95" s="10"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
       <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,54 +2590,64 @@
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
-      <c r="E96" s="10"/>
-      <c r="F96" s="10"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
       <c r="G96" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="I21:I28"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="I12:I19"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="J1:N2"/>
-    <mergeCell ref="I3:I10"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="M33:N33"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="I30:I37"/>
-    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="I39:I46"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
     <mergeCell ref="A49:I49"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="E8:F8"/>
@@ -2641,58 +2672,48 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="I39:I46"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E91:F91"/>
-    <mergeCell ref="E92:F92"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="E80:F80"/>
-    <mergeCell ref="E81:F81"/>
-    <mergeCell ref="E82:F82"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="M33:N33"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="I30:I37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="J1:N2"/>
+    <mergeCell ref="I3:I10"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="I21:I28"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="I12:I19"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>